<commit_message>
Mobile SiteInfo: materials inventory section revamp
- Generalize materials actions (materials-inventory), remove NPC-only filters
- Add catalog-driven dropdown (includes inactive inventory like NPC-9000)
- UI: unify dropdown radius/size, remove label, adjust spacing
- KPI: show selected material/unit, remove redundant '합계'
- Inventory preview list and improved logsheet header layout
- Logs: header simplified, chips gray tone; compact dropdown
- Bugfix: include active materials without inventory in dropdown
- Author dropdown: load site workers for selection in work log
</commit_message>
<xml_diff>
--- a/dy_memo/요청데이터_20251010/소속사-현장-mapping2.xlsx
+++ b/dy_memo/요청데이터_20251010/소속사-현장-mapping2.xlsx
@@ -8,14 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidyang/workspace/INOPNC_WM_20250829/dy_memo/요청데이터_20251010/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2320060E-0ACA-3443-BEF4-C06E81C32A36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A61C197A-F7BE-0C4E-9AE0-C7421FECAEF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25980" yWindow="7880" windowWidth="26200" windowHeight="21280" xr2:uid="{5718A82D-AE2F-864C-9F4B-DBBA0FC4A4BD}"/>
+    <workbookView xWindow="38160" yWindow="4160" windowWidth="18520" windowHeight="19420" activeTab="2" xr2:uid="{5718A82D-AE2F-864C-9F4B-DBBA0FC4A4BD}"/>
   </bookViews>
   <sheets>
-    <sheet name="소속사-현장-mapping" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId2"/>
+    <sheet name="소속사-현장-mapping" sheetId="1" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'소속사-현장-mapping'!$A$1:$B$61</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
+  <pivotCaches>
+    <pivotCache cacheId="10" r:id="rId4"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="76">
   <si>
     <t>소속사명</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -260,6 +268,12 @@
   </si>
   <si>
     <t>서대구힐스테이트</t>
+  </si>
+  <si>
+    <t>행 레이블</t>
+  </si>
+  <si>
+    <t>총합계</t>
   </si>
 </sst>
 </file>
@@ -328,7 +342,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -336,6 +350,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -352,6 +372,638 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="David Yang" refreshedDate="45954.427726967595" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="60" xr:uid="{A81893A2-D790-F548-B5EF-A7768B1B79C0}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:B61" sheet="소속사-현장-mapping"/>
+  </cacheSource>
+  <cacheFields count="2">
+    <cacheField name="소속사명" numFmtId="0">
+      <sharedItems count="12">
+        <s v="삼일"/>
+        <s v="KC산업"/>
+        <s v="SK하이닉스"/>
+        <s v="삼표피앤씨"/>
+        <s v="동부건설"/>
+        <s v="삼표산업"/>
+        <s v="지피씨"/>
+        <s v="한성PC"/>
+        <s v="아이에스동서"/>
+        <s v="우미건설"/>
+        <s v="케이씨산업"/>
+        <s v="한성"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="현장명" numFmtId="0">
+      <sharedItems count="60">
+        <s v="김포"/>
+        <s v="여주점봉"/>
+        <s v="커플러"/>
+        <s v="광주삼동"/>
+        <s v="용인왕산2블럭"/>
+        <s v="고향장항"/>
+        <s v="안성CDC물류센터"/>
+        <s v="동진PCE"/>
+        <s v="송도4차"/>
+        <s v="청주하이닉스"/>
+        <s v="동부건설 동탄 파크릭스"/>
+        <s v="울산샤인"/>
+        <s v="송도센터파크힐스테이트"/>
+        <s v="익산마동"/>
+        <s v="여주공장"/>
+        <s v="당진익산"/>
+        <s v="청량리 롯데건설"/>
+        <s v="공덕 자이"/>
+        <s v="김포케이원"/>
+        <s v="이천중리"/>
+        <s v="동탄파크릭스"/>
+        <s v="부산세그먼트"/>
+        <s v="송도2차및3차"/>
+        <s v="속초힐스"/>
+        <s v="부천일루미스테이트"/>
+        <s v="용인둔전힐스테이트"/>
+        <s v="잠실전력구"/>
+        <s v="화성봉담"/>
+        <s v="기타"/>
+        <s v="여수죽림2블럭 균열"/>
+        <s v="안성일죽동원물류"/>
+        <s v="용인 y1  IBL CUB"/>
+        <s v="파주운정GTX"/>
+        <s v="오산로지폴리스"/>
+        <s v="반포래미안"/>
+        <s v="인천주안힐스테이트"/>
+        <s v="창원더퍼스트"/>
+        <s v="대전도마"/>
+        <s v="대전도안리버파크"/>
+        <s v="디에이치방배"/>
+        <s v="이천공장"/>
+        <s v="포항환호공원2BL"/>
+        <s v="포항환호공원1BL"/>
+        <s v="일산현장"/>
+        <s v="국민대보건설시흥정왕행복주택"/>
+        <s v="개포1단지"/>
+        <s v="한성이천중리"/>
+        <s v="창원마크로엔"/>
+        <s v="용인Y1wwt"/>
+        <s v="세종가은마을"/>
+        <s v="영등포디그니티"/>
+        <s v="광주신용더리버"/>
+        <s v="순천덕암"/>
+        <s v="용인 y1  IBL CUB2"/>
+        <s v="당진힐스테이트"/>
+        <s v="테라시흥시청1차기성"/>
+        <s v="인천검단"/>
+        <s v="인천검단2"/>
+        <s v="힐스테이트레이크송도4차"/>
+        <s v="서대구힐스테이트"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="60">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="12"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="14"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="15"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="16"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="17"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="19"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="20"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="21"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="23"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="24"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="25"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="26"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="27"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="28"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="29"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="30"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="31"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="32"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="34"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="35"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="36"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="37"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="38"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="39"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="40"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="41"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="42"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="43"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="44"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="45"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="46"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="47"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="48"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="49"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="50"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="51"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="52"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="53"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="54"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="55"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="56"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="57"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="58"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="59"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{05337B28-008B-734D-9583-9DF12A4E1756}" name="피벗 테이블2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:A16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="13">
+        <item x="4"/>
+        <item x="0"/>
+        <item x="5"/>
+        <item x="3"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="6"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="7"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="61">
+        <item x="45"/>
+        <item x="5"/>
+        <item x="17"/>
+        <item x="3"/>
+        <item x="51"/>
+        <item x="44"/>
+        <item x="28"/>
+        <item x="0"/>
+        <item x="18"/>
+        <item x="15"/>
+        <item x="54"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="10"/>
+        <item x="7"/>
+        <item x="20"/>
+        <item x="39"/>
+        <item x="34"/>
+        <item x="21"/>
+        <item x="24"/>
+        <item x="59"/>
+        <item x="49"/>
+        <item x="23"/>
+        <item x="22"/>
+        <item x="8"/>
+        <item x="12"/>
+        <item x="52"/>
+        <item x="30"/>
+        <item x="6"/>
+        <item x="29"/>
+        <item x="14"/>
+        <item x="1"/>
+        <item x="50"/>
+        <item x="33"/>
+        <item x="31"/>
+        <item x="53"/>
+        <item x="25"/>
+        <item x="4"/>
+        <item x="48"/>
+        <item x="11"/>
+        <item x="40"/>
+        <item x="19"/>
+        <item x="13"/>
+        <item x="56"/>
+        <item x="57"/>
+        <item x="35"/>
+        <item x="43"/>
+        <item x="26"/>
+        <item x="36"/>
+        <item x="47"/>
+        <item x="16"/>
+        <item x="9"/>
+        <item x="2"/>
+        <item x="55"/>
+        <item x="32"/>
+        <item x="42"/>
+        <item x="41"/>
+        <item x="46"/>
+        <item x="27"/>
+        <item x="58"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="13">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DA2306EC-0FC5-5043-91A7-DEC6F37FFCD4}" name="피벗 테이블3" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:A16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField axis="axisRow" showAll="0" sortType="ascending">
+      <items count="13">
+        <item x="4"/>
+        <item x="0"/>
+        <item x="5"/>
+        <item x="3"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="6"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="7"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="61">
+        <item x="45"/>
+        <item x="5"/>
+        <item x="17"/>
+        <item x="3"/>
+        <item x="51"/>
+        <item x="44"/>
+        <item x="28"/>
+        <item x="0"/>
+        <item x="18"/>
+        <item x="15"/>
+        <item x="54"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="10"/>
+        <item x="7"/>
+        <item x="20"/>
+        <item x="39"/>
+        <item x="34"/>
+        <item x="21"/>
+        <item x="24"/>
+        <item x="59"/>
+        <item x="49"/>
+        <item x="23"/>
+        <item x="22"/>
+        <item x="8"/>
+        <item x="12"/>
+        <item x="52"/>
+        <item x="30"/>
+        <item x="6"/>
+        <item x="29"/>
+        <item x="14"/>
+        <item x="1"/>
+        <item x="50"/>
+        <item x="33"/>
+        <item x="31"/>
+        <item x="53"/>
+        <item x="25"/>
+        <item x="4"/>
+        <item x="48"/>
+        <item x="11"/>
+        <item x="40"/>
+        <item x="19"/>
+        <item x="13"/>
+        <item x="56"/>
+        <item x="57"/>
+        <item x="35"/>
+        <item x="43"/>
+        <item x="26"/>
+        <item x="36"/>
+        <item x="47"/>
+        <item x="16"/>
+        <item x="9"/>
+        <item x="2"/>
+        <item x="55"/>
+        <item x="32"/>
+        <item x="42"/>
+        <item x="41"/>
+        <item x="46"/>
+        <item x="27"/>
+        <item x="58"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="13">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -670,16 +1322,245 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A000F1-E5BC-4A47-A024-7DE0ADF4A289}">
-  <dimension ref="A1:B61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1397ECA0-D0AF-4E4B-954B-5F99CB8654E5}">
+  <dimension ref="A3:A16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
-    <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="41" max="45" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="50" max="51" width="12" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="12" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="57" max="58" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="12" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="6.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:1">
+      <c r="A3" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BE8CCB2-2228-6A40-ADC8-76498705941E}">
+  <dimension ref="A3:A16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:1">
+      <c r="A3" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A000F1-E5BC-4A47-A024-7DE0ADF4A289}">
+  <dimension ref="A1:B61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -692,10 +1573,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -703,79 +1584,79 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -783,7 +1664,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -791,7 +1672,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -799,7 +1680,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -807,7 +1688,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -815,31 +1696,31 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -847,7 +1728,7 @@
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -855,15 +1736,15 @@
         <v>5</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -871,15 +1752,15 @@
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -887,7 +1768,7 @@
         <v>5</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -895,15 +1776,15 @@
         <v>5</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -916,10 +1797,10 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -927,15 +1808,15 @@
         <v>5</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -943,7 +1824,7 @@
         <v>5</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -951,7 +1832,7 @@
         <v>5</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -959,23 +1840,23 @@
         <v>5</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -983,7 +1864,7 @@
         <v>5</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -991,7 +1872,7 @@
         <v>5</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -999,7 +1880,7 @@
         <v>5</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1007,15 +1888,15 @@
         <v>5</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1023,7 +1904,7 @@
         <v>5</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1031,23 +1912,23 @@
         <v>5</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1055,23 +1936,23 @@
         <v>5</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1079,98 +1960,103 @@
         <v>10</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="2" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="2" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>71</v>
+        <v>32</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>72</v>
+        <v>16</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>73</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B61" xr:uid="{76A000F1-E5BC-4A47-A024-7DE0ADF4A289}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B61">
+      <sortCondition ref="A1:A61"/>
+    </sortState>
+  </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>